<commit_message>
Datos actualizados en el archivo de prueba XLS
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyects\Read_XLS_with_PHP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39697C01-D599-459B-8878-279036D21AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,112 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>Jorge Emiliano Maldonado</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/JorgeEmilianoM</t>
+  </si>
+  <si>
+    <t>Silvia Manrique</t>
+  </si>
+  <si>
+    <t>behance.net/kittymanri5a4a</t>
+  </si>
+  <si>
+    <t>Portfolio.GesPrender.com</t>
+  </si>
+  <si>
+    <t>Anibal Niz</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/anibal-niz-56a3a2217/</t>
+  </si>
+  <si>
+    <t>github.com/AnibalNiz4</t>
+  </si>
+  <si>
+    <t>github.com/JorgeEmilianoM</t>
+  </si>
+  <si>
+    <t>JorgeEmilianoM@gmail.com</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/silvia-manrique-794931179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anibal.niz@hotmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaime Andrés Moncayo Parra </t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/jaime-andres-moncayo-parra-7407a512b/</t>
+  </si>
+  <si>
+    <t>github.com/jaime1315321</t>
+  </si>
+  <si>
+    <t>Dylan España</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/dylan-españa-c-200abc</t>
+  </si>
+  <si>
+    <t>github.com/DylanCerv</t>
+  </si>
+  <si>
+    <t>gownerbeats@gmail.com</t>
+  </si>
+  <si>
+    <t>jamoncayop@unal.edu.co</t>
+  </si>
+  <si>
+    <t>Víctor Olivera</t>
+  </si>
+  <si>
+    <t>ovictoriox@gmail.com</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/victor-olivera/</t>
+  </si>
+  <si>
+    <t>github.com/oliveravictor</t>
+  </si>
+  <si>
+    <t>Daniela Estefanía Moreán</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/daniela-moreán</t>
+  </si>
+  <si>
+    <t>estefaniamorean@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,13 +154,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +443,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{CA4E4BAF-6AA4-4DEB-A270-914FF8628764}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EA94062B-F25A-4277-83B3-36186CBB6ACE}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{D1992BB1-55DB-4462-AC2B-8EEFE65AAC53}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{5499193C-BD79-4092-AEC0-40D00692EF40}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{357EE3DE-16F7-410B-971A-9A192DA82696}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{E57FC745-B50F-4B75-A85E-BB326B7D1835}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>